<commit_message>
finished main features, need to clean UI and output
</commit_message>
<xml_diff>
--- a/sheets/County Time and Supplies Record.xlsx
+++ b/sheets/County Time and Supplies Record.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2745" yWindow="1200" windowWidth="21600" windowHeight="11385" tabRatio="907" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="2745" yWindow="1200" windowWidth="21600" windowHeight="11385" tabRatio="907" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Claims" sheetId="37" r:id="rId1"/>
@@ -1132,7 +1132,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3681,7 +3681,7 @@
   </sheetPr>
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
@@ -5058,7 +5058,7 @@
   </sheetPr>
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
       <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>

</xml_diff>